<commit_message>
added request - copy.xlsx
</commit_message>
<xml_diff>
--- a/Personal/Trajectories adhoc request.xlsx
+++ b/Personal/Trajectories adhoc request.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Performance</t>
   </si>
@@ -63,7 +63,10 @@
     <t xml:space="preserve">  group by month</t>
   </si>
   <si>
-    <t>how</t>
+    <t>Testing git ignore</t>
+  </si>
+  <si>
+    <t>Testing git ignore2</t>
   </si>
 </sst>
 </file>
@@ -439,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,6 +585,11 @@
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>